<commit_message>
update data source mappings and formats
</commit_message>
<xml_diff>
--- a/assets/majors.xlsx
+++ b/assets/majors.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alasw\Documents\UMich\MADS\Courses\SIADS - 593 Milestone 1\Project\Project\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{55A4D454-BA0B-4361-BEB4-38E71F18EDC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98AA2F77-3089-4D5F-AD9D-1A64DB3FAF6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="1110" windowWidth="21090" windowHeight="13190" xr2:uid="{8E3DFEB7-E3CC-4047-925A-F8240E372E2B}"/>
+    <workbookView xWindow="6420" yWindow="2740" windowWidth="28800" windowHeight="16320" xr2:uid="{8E3DFEB7-E3CC-4047-925A-F8240E372E2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$349</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="362">
   <si>
     <t>Business and financial operations occupations</t>
   </si>
@@ -1110,6 +1113,18 @@
   </si>
   <si>
     <t>Women's Studies BSChem</t>
+  </si>
+  <si>
+    <t>Architecture and engineering occupations</t>
+  </si>
+  <si>
+    <t>Community and social service occupations</t>
+  </si>
+  <si>
+    <t>Healthcare practitioners and technical occupations</t>
+  </si>
+  <si>
+    <t>Management occupations</t>
   </si>
 </sst>
 </file>
@@ -1125,18 +1140,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1151,9 +1160,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1494,8 +1502,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.26953125" customWidth="1"/>
+    <col min="2" max="2" width="71.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -1511,7 +1519,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1519,7 +1527,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1527,7 +1535,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -1535,7 +1543,7 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -1543,7 +1551,7 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -1551,7 +1559,7 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -1559,7 +1567,7 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -1567,7 +1575,7 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -1575,7 +1583,7 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -1583,7 +1591,7 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -1591,7 +1599,7 @@
         <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -1599,7 +1607,7 @@
         <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -1607,7 +1615,7 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -1615,7 +1623,7 @@
         <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -1623,7 +1631,7 @@
         <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -1631,7 +1639,7 @@
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -1719,7 +1727,7 @@
         <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
@@ -1727,7 +1735,7 @@
         <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -1735,25 +1743,31 @@
         <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>40</v>
       </c>
+      <c r="B31" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>41</v>
       </c>
+      <c r="B32" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>42</v>
       </c>
       <c r="B33" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
@@ -1761,7 +1775,7 @@
         <v>43</v>
       </c>
       <c r="B34" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -1769,7 +1783,7 @@
         <v>44</v>
       </c>
       <c r="B35" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -1777,7 +1791,7 @@
         <v>45</v>
       </c>
       <c r="B36" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -1785,7 +1799,7 @@
         <v>46</v>
       </c>
       <c r="B37" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
@@ -1793,7 +1807,7 @@
         <v>47</v>
       </c>
       <c r="B38" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
@@ -1801,7 +1815,7 @@
         <v>48</v>
       </c>
       <c r="B39" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
@@ -1809,7 +1823,7 @@
         <v>49</v>
       </c>
       <c r="B40" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
@@ -1817,7 +1831,7 @@
         <v>50</v>
       </c>
       <c r="B41" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
@@ -1825,7 +1839,7 @@
         <v>51</v>
       </c>
       <c r="B42" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
@@ -1833,7 +1847,7 @@
         <v>52</v>
       </c>
       <c r="B43" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
@@ -1841,7 +1855,7 @@
         <v>53</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
@@ -1849,7 +1863,7 @@
         <v>54</v>
       </c>
       <c r="B45" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
@@ -1857,7 +1871,7 @@
         <v>55</v>
       </c>
       <c r="B46" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
@@ -1865,7 +1879,7 @@
         <v>56</v>
       </c>
       <c r="B47" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
@@ -1873,7 +1887,7 @@
         <v>57</v>
       </c>
       <c r="B48" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
@@ -1881,7 +1895,7 @@
         <v>58</v>
       </c>
       <c r="B49" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
@@ -1889,7 +1903,7 @@
         <v>59</v>
       </c>
       <c r="B50" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
@@ -1905,7 +1919,7 @@
         <v>62</v>
       </c>
       <c r="B52" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
@@ -1913,7 +1927,7 @@
         <v>63</v>
       </c>
       <c r="B53" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
@@ -1921,20 +1935,23 @@
         <v>64</v>
       </c>
       <c r="B54" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>65</v>
       </c>
+      <c r="B55" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>66</v>
       </c>
       <c r="B56" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
@@ -1942,7 +1959,7 @@
         <v>67</v>
       </c>
       <c r="B57" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -1950,7 +1967,7 @@
         <v>68</v>
       </c>
       <c r="B58" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
@@ -1958,7 +1975,7 @@
         <v>69</v>
       </c>
       <c r="B59" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
@@ -1982,7 +1999,7 @@
         <v>72</v>
       </c>
       <c r="B62" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
@@ -1990,7 +2007,7 @@
         <v>73</v>
       </c>
       <c r="B63" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
@@ -2014,7 +2031,7 @@
         <v>76</v>
       </c>
       <c r="B66" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
@@ -2022,7 +2039,7 @@
         <v>77</v>
       </c>
       <c r="B67" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
@@ -2030,7 +2047,7 @@
         <v>78</v>
       </c>
       <c r="B68" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
@@ -2054,7 +2071,7 @@
         <v>81</v>
       </c>
       <c r="B71" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
@@ -2062,7 +2079,7 @@
         <v>82</v>
       </c>
       <c r="B72" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
@@ -2070,7 +2087,7 @@
         <v>83</v>
       </c>
       <c r="B73" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
@@ -2078,7 +2095,7 @@
         <v>84</v>
       </c>
       <c r="B74" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
@@ -2126,7 +2143,7 @@
         <v>90</v>
       </c>
       <c r="B80" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
@@ -2166,7 +2183,7 @@
         <v>95</v>
       </c>
       <c r="B85" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
@@ -2174,7 +2191,7 @@
         <v>96</v>
       </c>
       <c r="B86" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
@@ -2182,7 +2199,7 @@
         <v>97</v>
       </c>
       <c r="B87" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
@@ -2213,11 +2230,17 @@
       <c r="A91" t="s">
         <v>101</v>
       </c>
+      <c r="B91" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>102</v>
       </c>
+      <c r="B92" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
@@ -2256,7 +2279,7 @@
         <v>107</v>
       </c>
       <c r="B97" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
@@ -2264,7 +2287,7 @@
         <v>108</v>
       </c>
       <c r="B98" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
@@ -2272,7 +2295,7 @@
         <v>109</v>
       </c>
       <c r="B99" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
@@ -2280,7 +2303,7 @@
         <v>110</v>
       </c>
       <c r="B100" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
@@ -2288,7 +2311,7 @@
         <v>111</v>
       </c>
       <c r="B101" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
@@ -2296,7 +2319,7 @@
         <v>112</v>
       </c>
       <c r="B102" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
@@ -2304,7 +2327,7 @@
         <v>113</v>
       </c>
       <c r="B103" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
@@ -2312,7 +2335,7 @@
         <v>114</v>
       </c>
       <c r="B104" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
@@ -2320,7 +2343,7 @@
         <v>115</v>
       </c>
       <c r="B105" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
@@ -2360,7 +2383,7 @@
         <v>120</v>
       </c>
       <c r="B110" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
@@ -2368,7 +2391,7 @@
         <v>121</v>
       </c>
       <c r="B111" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
@@ -2376,7 +2399,7 @@
         <v>122</v>
       </c>
       <c r="B112" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
@@ -2384,7 +2407,7 @@
         <v>123</v>
       </c>
       <c r="B113" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
@@ -2392,7 +2415,7 @@
         <v>124</v>
       </c>
       <c r="B114" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
@@ -2400,7 +2423,7 @@
         <v>125</v>
       </c>
       <c r="B115" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
@@ -2408,7 +2431,7 @@
         <v>126</v>
       </c>
       <c r="B116" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
@@ -2416,7 +2439,7 @@
         <v>127</v>
       </c>
       <c r="B117" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
@@ -2424,7 +2447,7 @@
         <v>128</v>
       </c>
       <c r="B118" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
@@ -2432,7 +2455,7 @@
         <v>129</v>
       </c>
       <c r="B119" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
@@ -2440,7 +2463,7 @@
         <v>130</v>
       </c>
       <c r="B120" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
@@ -2448,7 +2471,7 @@
         <v>131</v>
       </c>
       <c r="B121" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
@@ -2456,7 +2479,7 @@
         <v>132</v>
       </c>
       <c r="B122" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
@@ -2464,7 +2487,7 @@
         <v>133</v>
       </c>
       <c r="B123" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
@@ -2512,7 +2535,7 @@
         <v>139</v>
       </c>
       <c r="B129" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
@@ -2520,7 +2543,7 @@
         <v>140</v>
       </c>
       <c r="B130" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
@@ -2528,7 +2551,7 @@
         <v>141</v>
       </c>
       <c r="B131" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
@@ -2536,7 +2559,7 @@
         <v>142</v>
       </c>
       <c r="B132" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
@@ -2559,6 +2582,9 @@
       <c r="A135" t="s">
         <v>145</v>
       </c>
+      <c r="B135" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
@@ -2597,7 +2623,7 @@
         <v>150</v>
       </c>
       <c r="B140" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
@@ -2605,7 +2631,7 @@
         <v>151</v>
       </c>
       <c r="B141" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
@@ -2613,7 +2639,7 @@
         <v>152</v>
       </c>
       <c r="B142" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
@@ -2637,7 +2663,7 @@
         <v>155</v>
       </c>
       <c r="B145" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
@@ -2645,7 +2671,7 @@
         <v>156</v>
       </c>
       <c r="B146" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
@@ -2772,25 +2798,31 @@
       <c r="A162" t="s">
         <v>173</v>
       </c>
+      <c r="B162" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>174</v>
       </c>
+      <c r="B163" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>175</v>
       </c>
       <c r="B164" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>176</v>
       </c>
-      <c r="B165" s="1" t="s">
+      <c r="B165" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2798,7 +2830,7 @@
       <c r="A166" t="s">
         <v>177</v>
       </c>
-      <c r="B166" s="1" t="s">
+      <c r="B166" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2839,7 +2871,7 @@
         <v>182</v>
       </c>
       <c r="B171" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
@@ -2847,7 +2879,7 @@
         <v>183</v>
       </c>
       <c r="B172" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
@@ -2855,7 +2887,7 @@
         <v>184</v>
       </c>
       <c r="B173" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
@@ -2863,7 +2895,7 @@
         <v>185</v>
       </c>
       <c r="B174" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
@@ -2871,7 +2903,7 @@
         <v>186</v>
       </c>
       <c r="B175" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
@@ -2887,7 +2919,7 @@
         <v>188</v>
       </c>
       <c r="B177" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
@@ -2895,7 +2927,7 @@
         <v>189</v>
       </c>
       <c r="B178" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
@@ -2935,7 +2967,7 @@
         <v>194</v>
       </c>
       <c r="B183" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
@@ -2943,7 +2975,7 @@
         <v>195</v>
       </c>
       <c r="B184" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
@@ -2951,7 +2983,7 @@
         <v>196</v>
       </c>
       <c r="B185" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
@@ -2959,7 +2991,7 @@
         <v>197</v>
       </c>
       <c r="B186" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
@@ -2967,7 +2999,7 @@
         <v>198</v>
       </c>
       <c r="B187" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
@@ -2975,7 +3007,7 @@
         <v>199</v>
       </c>
       <c r="B188" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
@@ -2983,7 +3015,7 @@
         <v>200</v>
       </c>
       <c r="B189" t="s">
-        <v>1</v>
+        <v>360</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
@@ -2999,7 +3031,7 @@
         <v>202</v>
       </c>
       <c r="B191" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
@@ -3007,7 +3039,7 @@
         <v>203</v>
       </c>
       <c r="B192" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
@@ -3031,7 +3063,7 @@
         <v>206</v>
       </c>
       <c r="B195" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
@@ -3063,7 +3095,7 @@
         <v>210</v>
       </c>
       <c r="B199" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
@@ -3071,7 +3103,7 @@
         <v>211</v>
       </c>
       <c r="B200" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
@@ -3103,7 +3135,7 @@
         <v>215</v>
       </c>
       <c r="B204" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
@@ -3119,7 +3151,7 @@
         <v>217</v>
       </c>
       <c r="B206" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.35">
@@ -3151,7 +3183,7 @@
         <v>221</v>
       </c>
       <c r="B210" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.35">
@@ -3159,7 +3191,7 @@
         <v>222</v>
       </c>
       <c r="B211" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
@@ -3167,7 +3199,7 @@
         <v>223</v>
       </c>
       <c r="B212" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.35">
@@ -3175,7 +3207,7 @@
         <v>224</v>
       </c>
       <c r="B213" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.35">
@@ -3207,7 +3239,7 @@
         <v>228</v>
       </c>
       <c r="B217" t="s">
-        <v>172</v>
+        <v>1</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.35">
@@ -3215,7 +3247,7 @@
         <v>229</v>
       </c>
       <c r="B218" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.35">
@@ -3319,7 +3351,7 @@
         <v>242</v>
       </c>
       <c r="B231" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.35">
@@ -3343,7 +3375,7 @@
         <v>245</v>
       </c>
       <c r="B234" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.35">
@@ -3351,7 +3383,7 @@
         <v>246</v>
       </c>
       <c r="B235" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.35">
@@ -3359,7 +3391,7 @@
         <v>247</v>
       </c>
       <c r="B236" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.35">
@@ -3367,7 +3399,7 @@
         <v>248</v>
       </c>
       <c r="B237" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.35">
@@ -3375,7 +3407,7 @@
         <v>249</v>
       </c>
       <c r="B238" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.35">
@@ -3383,7 +3415,7 @@
         <v>250</v>
       </c>
       <c r="B239" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.35">
@@ -3391,7 +3423,7 @@
         <v>251</v>
       </c>
       <c r="B240" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.35">
@@ -3399,7 +3431,7 @@
         <v>252</v>
       </c>
       <c r="B241" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.35">
@@ -3407,7 +3439,7 @@
         <v>253</v>
       </c>
       <c r="B242" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.35">
@@ -3415,7 +3447,7 @@
         <v>254</v>
       </c>
       <c r="B243" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.35">
@@ -3423,7 +3455,7 @@
         <v>255</v>
       </c>
       <c r="B244" t="s">
-        <v>6</v>
+        <v>172</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.35">
@@ -3431,7 +3463,7 @@
         <v>256</v>
       </c>
       <c r="B245" t="s">
-        <v>6</v>
+        <v>172</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.35">
@@ -3439,7 +3471,7 @@
         <v>257</v>
       </c>
       <c r="B246" t="s">
-        <v>6</v>
+        <v>172</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.35">
@@ -3447,7 +3479,7 @@
         <v>258</v>
       </c>
       <c r="B247" t="s">
-        <v>6</v>
+        <v>172</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.35">
@@ -3455,7 +3487,7 @@
         <v>259</v>
       </c>
       <c r="B248" t="s">
-        <v>6</v>
+        <v>172</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.35">
@@ -3463,7 +3495,7 @@
         <v>260</v>
       </c>
       <c r="B249" t="s">
-        <v>6</v>
+        <v>172</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.35">
@@ -3471,7 +3503,7 @@
         <v>261</v>
       </c>
       <c r="B250" t="s">
-        <v>6</v>
+        <v>172</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.35">
@@ -3543,7 +3575,7 @@
         <v>269</v>
       </c>
       <c r="B259" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.35">
@@ -3551,7 +3583,7 @@
         <v>270</v>
       </c>
       <c r="B260" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.35">
@@ -3559,7 +3591,7 @@
         <v>271</v>
       </c>
       <c r="B261" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.35">
@@ -3567,7 +3599,7 @@
         <v>272</v>
       </c>
       <c r="B262" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.35">
@@ -3583,7 +3615,7 @@
         <v>274</v>
       </c>
       <c r="B264" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.35">
@@ -3591,7 +3623,7 @@
         <v>275</v>
       </c>
       <c r="B265" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.35">
@@ -3599,7 +3631,7 @@
         <v>276</v>
       </c>
       <c r="B266" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.35">
@@ -3607,7 +3639,7 @@
         <v>277</v>
       </c>
       <c r="B267" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.35">
@@ -3615,7 +3647,7 @@
         <v>278</v>
       </c>
       <c r="B268" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.35">
@@ -3623,7 +3655,7 @@
         <v>279</v>
       </c>
       <c r="B269" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.35">
@@ -3631,7 +3663,7 @@
         <v>280</v>
       </c>
       <c r="B270" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.35">
@@ -3719,7 +3751,7 @@
         <v>291</v>
       </c>
       <c r="B281" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.35">
@@ -3727,7 +3759,7 @@
         <v>292</v>
       </c>
       <c r="B282" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.35">
@@ -3735,7 +3767,7 @@
         <v>293</v>
       </c>
       <c r="B283" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.35">
@@ -3743,7 +3775,7 @@
         <v>294</v>
       </c>
       <c r="B284" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.35">
@@ -3751,7 +3783,7 @@
         <v>295</v>
       </c>
       <c r="B285" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.35">
@@ -3759,7 +3791,7 @@
         <v>296</v>
       </c>
       <c r="B286" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.35">
@@ -3767,7 +3799,7 @@
         <v>297</v>
       </c>
       <c r="B287" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.35">
@@ -3775,7 +3807,7 @@
         <v>298</v>
       </c>
       <c r="B288" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.35">
@@ -3783,7 +3815,7 @@
         <v>299</v>
       </c>
       <c r="B289" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.35">
@@ -3791,14 +3823,14 @@
         <v>300</v>
       </c>
       <c r="B290" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
         <v>301</v>
       </c>
-      <c r="B291" s="1" t="s">
+      <c r="B291" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3807,7 +3839,7 @@
         <v>302</v>
       </c>
       <c r="B292" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.35">
@@ -3815,7 +3847,7 @@
         <v>303</v>
       </c>
       <c r="B293" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
@@ -3823,7 +3855,7 @@
         <v>304</v>
       </c>
       <c r="B294" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.35">
@@ -3831,7 +3863,7 @@
         <v>305</v>
       </c>
       <c r="B295" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.35">
@@ -3839,7 +3871,7 @@
         <v>306</v>
       </c>
       <c r="B296" t="s">
-        <v>1</v>
+        <v>361</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.35">
@@ -3847,7 +3879,7 @@
         <v>307</v>
       </c>
       <c r="B297" t="s">
-        <v>1</v>
+        <v>361</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.35">
@@ -3951,7 +3983,7 @@
         <v>320</v>
       </c>
       <c r="B310" t="s">
-        <v>6</v>
+        <v>172</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.35">
@@ -4031,7 +4063,7 @@
         <v>330</v>
       </c>
       <c r="B320" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.35">
@@ -4111,7 +4143,7 @@
         <v>339</v>
       </c>
       <c r="B330" t="s">
-        <v>1</v>
+        <v>359</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.35">
@@ -4119,7 +4151,7 @@
         <v>340</v>
       </c>
       <c r="B331" t="s">
-        <v>1</v>
+        <v>359</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.35">
@@ -4135,7 +4167,7 @@
         <v>342</v>
       </c>
       <c r="B333" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.35">
@@ -4143,7 +4175,7 @@
         <v>343</v>
       </c>
       <c r="B334" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.35">
@@ -4151,7 +4183,7 @@
         <v>344</v>
       </c>
       <c r="B335" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.35">
@@ -4159,7 +4191,7 @@
         <v>345</v>
       </c>
       <c r="B336" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.35">
@@ -4167,7 +4199,7 @@
         <v>346</v>
       </c>
       <c r="B337" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.35">
@@ -4175,7 +4207,7 @@
         <v>347</v>
       </c>
       <c r="B338" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.35">
@@ -4183,7 +4215,7 @@
         <v>348</v>
       </c>
       <c r="B339" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.35">
@@ -4191,7 +4223,7 @@
         <v>349</v>
       </c>
       <c r="B340" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.35">
@@ -4238,13 +4270,16 @@
       <c r="A346" t="s">
         <v>5</v>
       </c>
+      <c r="B346" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A347" t="s">
         <v>355</v>
       </c>
       <c r="B347" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.35">
@@ -4252,7 +4287,7 @@
         <v>356</v>
       </c>
       <c r="B348" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.35">
@@ -4260,10 +4295,11 @@
         <v>357</v>
       </c>
       <c r="B349" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B349" xr:uid="{98D1733D-F13D-4CB6-83C4-5BC8897837CD}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
anthropology majors mapping edit
</commit_message>
<xml_diff>
--- a/assets/majors.xlsx
+++ b/assets/majors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alasw\Documents\UMich\MADS\Courses\SIADS - 593 Milestone 1\Project\Project\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98AA2F77-3089-4D5F-AD9D-1A64DB3FAF6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA70F9C-C627-4416-A222-D4365D55D26A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6420" yWindow="2740" windowWidth="28800" windowHeight="16320" xr2:uid="{8E3DFEB7-E3CC-4047-925A-F8240E372E2B}"/>
+    <workbookView xWindow="40320" yWindow="12390" windowWidth="17320" windowHeight="16320" xr2:uid="{8E3DFEB7-E3CC-4047-925A-F8240E372E2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1575,7 +1575,7 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -1583,7 +1583,7 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -1591,7 +1591,7 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -1599,7 +1599,7 @@
         <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -1607,7 +1607,7 @@
         <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
update merge_record merge joiner
</commit_message>
<xml_diff>
--- a/assets/majors.xlsx
+++ b/assets/majors.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alasw\Documents\UMich\MADS\Courses\SIADS - 593 Milestone 1\Project\Project\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA70F9C-C627-4416-A222-D4365D55D26A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D0A366-D5BC-4230-A704-993F529574DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40320" yWindow="12390" windowWidth="17320" windowHeight="16320" xr2:uid="{8E3DFEB7-E3CC-4047-925A-F8240E372E2B}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="21820" windowHeight="37900" xr2:uid="{8E3DFEB7-E3CC-4047-925A-F8240E372E2B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="majors" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$349</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">majors!$A$1:$B$349</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1498,7 +1498,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D1733D-F13D-4CB6-83C4-5BC8897837CD}">
   <dimension ref="A1:B349"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>